<commit_message>
revomed register panel and updated all user panels
</commit_message>
<xml_diff>
--- a/data/start_bosganlar.xlsx
+++ b/data/start_bosganlar.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,22 +482,22 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>6603133238</t>
+          <t>8208026680</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>PhD Tv admin</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>@phd_tv_admin</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-19</t>
         </is>
       </c>
     </row>
@@ -507,20 +507,45 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
+          <t>6603133238</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
           <t>2122000467</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Шавкат Рихситуллаев</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>@Shavkat630</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>2026-02-17</t>
         </is>

</xml_diff>